<commit_message>
Job parser and tweaks
</commit_message>
<xml_diff>
--- a/HPA/job.xlsx
+++ b/HPA/job.xlsx
@@ -17,27 +17,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>BrandName</t>
-  </si>
-  <si>
-    <t>BrandLocation</t>
-  </si>
-  <si>
-    <t>Hecs</t>
-  </si>
-  <si>
-    <t>Cuisine</t>
-  </si>
-  <si>
-    <t>BusinessEmail</t>
-  </si>
-  <si>
-    <t>GroupName</t>
-  </si>
-  <si>
-    <t>Media</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>experience</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>availability</t>
+  </si>
+  <si>
+    <t>startTime</t>
+  </si>
+  <si>
+    <t>compensation</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>openCall</t>
+  </si>
+  <si>
+    <t>interviewQuestion</t>
+  </si>
+  <si>
+    <t>trackingUrl</t>
+  </si>
+  <si>
+    <t>schedule</t>
+  </si>
+  <si>
+    <t>skill1|skill2|skill3|skill4</t>
+  </si>
+  <si>
+    <t>part|full|anytime</t>
   </si>
 </sst>
 </file>
@@ -379,7 +403,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,6 +420,7 @@
     <col min="10" max="10" width="17.5703125" customWidth="1"/>
     <col min="11" max="11" width="28.140625" customWidth="1"/>
     <col min="12" max="12" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -420,8 +445,45 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>123123</v>
+      </c>
+      <c r="B2">
+        <v>131</v>
+      </c>
+      <c r="C2">
+        <v>132312</v>
+      </c>
+      <c r="D2">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25"/>

</xml_diff>